<commit_message>
✨ automatic mainWindows construction
</commit_message>
<xml_diff>
--- a/Austerlitz.xlsx
+++ b/Austerlitz.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="94">
   <si>
     <t xml:space="preserve">Armee</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">moral</t>
   </si>
   <si>
+    <t xml:space="preserve">portrait</t>
+  </si>
+  <si>
     <t xml:space="preserve">fr</t>
   </si>
   <si>
@@ -133,27 +136,45 @@
     <t xml:space="preserve">Batterie Lourde réduite</t>
   </si>
   <si>
-    <t xml:space="preserve">NAPOLEON 1er</t>
+    <t xml:space="preserve">Napoleon</t>
   </si>
   <si>
     <t xml:space="preserve">generaux</t>
   </si>
   <si>
+    <t xml:space="preserve">Napoleon.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">BERNADOTE</t>
   </si>
   <si>
+    <t xml:space="preserve">Bernadotte.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">DAVOUT</t>
   </si>
   <si>
+    <t xml:space="preserve">Davout.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">SOULT</t>
   </si>
   <si>
+    <t xml:space="preserve">Soult.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">LANNES</t>
   </si>
   <si>
+    <t xml:space="preserve">Lannes.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">MURAT</t>
   </si>
   <si>
+    <t xml:space="preserve">Murat.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">au-ru</t>
   </si>
   <si>
@@ -250,19 +271,37 @@
     <t xml:space="preserve">ALEXANDRE Ier</t>
   </si>
   <si>
+    <t xml:space="preserve">AlexandreIer.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">BUXHOVEN</t>
   </si>
   <si>
+    <t xml:space="preserve">Buxhoevden.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">KOUTOUZOF</t>
   </si>
   <si>
+    <t xml:space="preserve">Koutouzof.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">BAGRATION</t>
   </si>
   <si>
+    <t xml:space="preserve">Bagration.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIECHTEINSTEIN</t>
   </si>
   <si>
+    <t xml:space="preserve">Liechtenstein.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">FRANCOIS II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RussiaFlag.jpg</t>
   </si>
 </sst>
 </file>
@@ -277,6 +316,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -358,13 +398,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I61" activeCellId="0" sqref="I33:I61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L65" activeCellId="0" sqref="L65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.97"/>
@@ -372,6 +412,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="4.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="4.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -402,16 +443,19 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -434,13 +478,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -463,13 +507,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -492,13 +536,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -521,13 +565,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>2</v>
@@ -550,13 +594,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>2</v>
@@ -579,13 +623,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>2</v>
@@ -608,13 +652,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>2</v>
@@ -637,13 +681,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>2</v>
@@ -666,13 +710,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>2</v>
@@ -695,13 +739,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>2</v>
@@ -724,13 +768,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>2</v>
@@ -753,13 +797,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>2</v>
@@ -782,13 +826,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2</v>
@@ -811,13 +855,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>2</v>
@@ -840,13 +884,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>2.5</v>
@@ -869,13 +913,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>2.5</v>
@@ -898,13 +942,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>5</v>
@@ -927,13 +971,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>0</v>
@@ -956,13 +1000,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0</v>
@@ -985,13 +1029,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>31</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0</v>
@@ -1014,13 +1058,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0</v>
@@ -1043,13 +1087,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>0</v>
@@ -1072,13 +1116,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>0</v>
@@ -1101,13 +1145,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>0</v>
@@ -1130,13 +1174,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>0</v>
@@ -1156,16 +1200,19 @@
       <c r="I27" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="J27" s="0" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>0</v>
@@ -1185,16 +1232,19 @@
       <c r="I28" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="J28" s="0" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>0</v>
@@ -1214,16 +1264,19 @@
       <c r="I29" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="J29" s="0" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>0</v>
@@ -1243,16 +1296,19 @@
       <c r="I30" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="J30" s="0" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>0</v>
@@ -1272,16 +1328,19 @@
       <c r="I31" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="J31" s="0" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>0</v>
@@ -1301,16 +1360,19 @@
       <c r="I32" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="J32" s="0" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>1</v>
@@ -1333,13 +1395,13 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>1</v>
@@ -1362,13 +1424,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>1</v>
@@ -1391,13 +1453,13 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>1</v>
@@ -1420,13 +1482,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>1</v>
@@ -1449,13 +1511,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>1</v>
@@ -1478,13 +1540,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>2</v>
@@ -1507,13 +1569,13 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>2</v>
@@ -1536,13 +1598,13 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>2</v>
@@ -1565,13 +1627,13 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>2</v>
@@ -1594,13 +1656,13 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>2</v>
@@ -1623,13 +1685,13 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>2</v>
@@ -1652,13 +1714,13 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>2</v>
@@ -1681,13 +1743,13 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>2</v>
@@ -1710,13 +1772,13 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>2</v>
@@ -1739,13 +1801,13 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>2</v>
@@ -1768,13 +1830,13 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>2</v>
@@ -1797,13 +1859,13 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>2.5</v>
@@ -1826,13 +1888,13 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>2.5</v>
@@ -1855,13 +1917,13 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>4</v>
@@ -1884,13 +1946,13 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>6</v>
@@ -1913,13 +1975,13 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>0</v>
@@ -1942,13 +2004,13 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>0</v>
@@ -1971,13 +2033,13 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>0</v>
@@ -2000,13 +2062,13 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>0</v>
@@ -2029,13 +2091,13 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>0</v>
@@ -2058,13 +2120,13 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>0</v>
@@ -2087,13 +2149,13 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>0</v>
@@ -2116,13 +2178,13 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>0</v>
@@ -2145,13 +2207,13 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>0</v>
@@ -2174,13 +2236,13 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>0</v>
@@ -2200,16 +2262,19 @@
       <c r="I63" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="J63" s="0" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>0</v>
@@ -2229,16 +2294,19 @@
       <c r="I64" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="J64" s="0" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>0</v>
@@ -2258,16 +2326,19 @@
       <c r="I65" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="J65" s="0" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>0</v>
@@ -2287,16 +2358,19 @@
       <c r="I66" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="J66" s="0" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>0</v>
@@ -2316,16 +2390,19 @@
       <c r="I67" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="J67" s="0" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>0</v>
@@ -2344,6 +2421,9 @@
       </c>
       <c r="I68" s="0" t="n">
         <v>0.5</v>
+      </c>
+      <c r="J68" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
💄 finalize troops selection
</commit_message>
<xml_diff>
--- a/Austerlitz.xlsx
+++ b/Austerlitz.xlsx
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="162">
   <si>
     <t xml:space="preserve">Armee</t>
   </si>
   <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
     <t xml:space="preserve">Troupe</t>
   </si>
   <si>
@@ -55,87 +58,165 @@
     <t xml:space="preserve">fr</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR01</t>
+  </si>
+  <si>
     <t xml:space="preserve">régiment(s) d'infanterie affaiblie</t>
   </si>
   <si>
-    <t xml:space="preserve">troupe</t>
+    <t xml:space="preserve">troupes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRTR02</t>
   </si>
   <si>
     <t xml:space="preserve">régiment(s) d'infanterie lègère</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR03</t>
+  </si>
+  <si>
     <t xml:space="preserve">régiment(s) d'infanterie de Ligne</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR04</t>
+  </si>
+  <si>
     <t xml:space="preserve">régiment(s) de Grenadiers</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR05</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brigade légère avec Legrand</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR06</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brigade de Ligne avec Général</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR07</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brigade de Grenadiers avec Duroc</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR08</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vieille Garde avec Bessière</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR09</t>
+  </si>
+  <si>
     <t xml:space="preserve">division(s) de cavalerie affaiblie</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR10</t>
+  </si>
+  <si>
     <t xml:space="preserve">division(s) de hussards</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR11</t>
+  </si>
+  <si>
     <t xml:space="preserve">division(s) de chasseurs</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR12</t>
+  </si>
+  <si>
     <t xml:space="preserve">division(s) de dragons</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR13</t>
+  </si>
+  <si>
     <t xml:space="preserve">division(s) de cuirassiers</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR14</t>
+  </si>
+  <si>
     <t xml:space="preserve">Div. de dragons de Walter</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR15</t>
+  </si>
+  <si>
     <t xml:space="preserve">Grenadiers à cheval</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR16</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cuirassiers avec MURAT</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR17</t>
+  </si>
+  <si>
     <t xml:space="preserve">batterie d'artillerie légère</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR18</t>
+  </si>
+  <si>
     <t xml:space="preserve">batterie d'artillerie Lourde</t>
   </si>
   <si>
+    <t xml:space="preserve">FRTR19</t>
+  </si>
+  <si>
     <t xml:space="preserve">Quartier Général</t>
   </si>
   <si>
+    <t xml:space="preserve">FRAR01</t>
+  </si>
+  <si>
     <t xml:space="preserve">1ere Batterie légère</t>
   </si>
   <si>
-    <t xml:space="preserve">artillerie</t>
+    <t xml:space="preserve">artilleries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRAR02</t>
   </si>
   <si>
     <t xml:space="preserve">2eme Batterie légère</t>
   </si>
   <si>
+    <t xml:space="preserve">FRAR03</t>
+  </si>
+  <si>
     <t xml:space="preserve">Batterie légère réduite</t>
   </si>
   <si>
+    <t xml:space="preserve">FRAR04</t>
+  </si>
+  <si>
     <t xml:space="preserve">1ere Batterie Lourde</t>
   </si>
   <si>
+    <t xml:space="preserve">FRAR05</t>
+  </si>
+  <si>
     <t xml:space="preserve">2eme Batterie Lourde</t>
   </si>
   <si>
+    <t xml:space="preserve">FRAR06</t>
+  </si>
+  <si>
     <t xml:space="preserve">Batterie Lourde réduite</t>
   </si>
   <si>
+    <t xml:space="preserve">FRGN01</t>
+  </si>
+  <si>
     <t xml:space="preserve">Napoleon</t>
   </si>
   <si>
@@ -145,30 +226,45 @@
     <t xml:space="preserve">Napoleon.webp</t>
   </si>
   <si>
+    <t xml:space="preserve">FRGN02</t>
+  </si>
+  <si>
     <t xml:space="preserve">BERNADOTE</t>
   </si>
   <si>
     <t xml:space="preserve">Bernadotte.jpg</t>
   </si>
   <si>
+    <t xml:space="preserve">FRGN03</t>
+  </si>
+  <si>
     <t xml:space="preserve">DAVOUT</t>
   </si>
   <si>
     <t xml:space="preserve">Davout.jpg</t>
   </si>
   <si>
+    <t xml:space="preserve">FRGN04</t>
+  </si>
+  <si>
     <t xml:space="preserve">SOULT</t>
   </si>
   <si>
     <t xml:space="preserve">Soult.jpg</t>
   </si>
   <si>
+    <t xml:space="preserve">FRGN05</t>
+  </si>
+  <si>
     <t xml:space="preserve">LANNES</t>
   </si>
   <si>
     <t xml:space="preserve">Lannes.jpg</t>
   </si>
   <si>
+    <t xml:space="preserve">FRGN06</t>
+  </si>
+  <si>
     <t xml:space="preserve">MURAT</t>
   </si>
   <si>
@@ -178,124 +274,232 @@
     <t xml:space="preserve">au-ru</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR01</t>
+  </si>
+  <si>
     <t xml:space="preserve">schwächregiment (rég. affaibli)</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR02</t>
+  </si>
+  <si>
     <t xml:space="preserve">landwerregiment(en) (milice)</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR03</t>
+  </si>
+  <si>
     <t xml:space="preserve">iéguerski (regiment de chasseurs)</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR04</t>
+  </si>
+  <si>
     <t xml:space="preserve">piéchoti (rég. de mousquetaires)</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR05</t>
+  </si>
+  <si>
     <t xml:space="preserve">grenadierregiment(en)</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR06</t>
+  </si>
+  <si>
     <t xml:space="preserve">piérota Proviti (reg. de la garde)</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR07</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jägerbrigade mit gl. Kienmayer</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR08</t>
+  </si>
+  <si>
     <t xml:space="preserve">Piéchoti y Vojd (Mousq. , Général )</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR09</t>
+  </si>
+  <si>
     <t xml:space="preserve">Grenadierbrigade mit gl. Kollowrath</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Piérota Proviti (Garde) y Constantin</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR11</t>
+  </si>
+  <si>
     <t xml:space="preserve">schwätchekavallerie (cav.affaiblie)</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR12</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hussardivision(en), Kosack</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR13</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dragouski (division de dragons)</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR14</t>
+  </si>
+  <si>
     <t xml:space="preserve">Arotnik Proviti (Ulhan de la Garde)</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR15</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hussarendivision mit general</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR16</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kosack Proviti y vojd Kologrivof</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR17</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dragouski Proviti (Chevalier-Garde)</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR18</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kurassieren mit LIECHENSTEIN</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR19</t>
+  </si>
+  <si>
     <t xml:space="preserve">leichartillerieshlägerei (art.légère)</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR20</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pouchka tiazholy (artillerie lourde)</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR21</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pouchka Pavlovskaia (art. de Pavlov)</t>
   </si>
   <si>
+    <t xml:space="preserve">ARTR22</t>
+  </si>
+  <si>
     <t xml:space="preserve">Haupquartier ( QG )</t>
   </si>
   <si>
+    <t xml:space="preserve">ARAR01</t>
+  </si>
+  <si>
     <t xml:space="preserve">leichartillerie A</t>
   </si>
   <si>
+    <t xml:space="preserve">ARAR02</t>
+  </si>
+  <si>
     <t xml:space="preserve">leichartillerie B</t>
   </si>
   <si>
+    <t xml:space="preserve">ARAR03</t>
+  </si>
+  <si>
     <t xml:space="preserve">1/2 leichartartillerie</t>
   </si>
   <si>
+    <t xml:space="preserve">ARAR04</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pouchka tiazholy A</t>
   </si>
   <si>
+    <t xml:space="preserve">ARAR05</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pouchka tiazholy B</t>
   </si>
   <si>
+    <t xml:space="preserve">ARAR06</t>
+  </si>
+  <si>
     <t xml:space="preserve">1/2 Pouchka tiazholy</t>
   </si>
   <si>
+    <t xml:space="preserve">ARAR07</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pouchka Pavloskaia</t>
   </si>
   <si>
+    <t xml:space="preserve">ARAR08</t>
+  </si>
+  <si>
     <t xml:space="preserve">1/2 Pouchka Pavloskaia</t>
   </si>
   <si>
+    <t xml:space="preserve">ARGN01</t>
+  </si>
+  <si>
     <t xml:space="preserve">ALEXANDRE Ier</t>
   </si>
   <si>
     <t xml:space="preserve">AlexandreIer.jpg</t>
   </si>
   <si>
+    <t xml:space="preserve">ARGN02</t>
+  </si>
+  <si>
     <t xml:space="preserve">BUXHOVEN</t>
   </si>
   <si>
     <t xml:space="preserve">Buxhoevden.jpg</t>
   </si>
   <si>
+    <t xml:space="preserve">ARGN03</t>
+  </si>
+  <si>
     <t xml:space="preserve">KOUTOUZOF</t>
   </si>
   <si>
     <t xml:space="preserve">Koutouzof.jpg</t>
   </si>
   <si>
+    <t xml:space="preserve">ARGN04</t>
+  </si>
+  <si>
     <t xml:space="preserve">BAGRATION</t>
   </si>
   <si>
     <t xml:space="preserve">Bagration.jpg</t>
   </si>
   <si>
+    <t xml:space="preserve">ARGN05</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIECHTEINSTEIN</t>
   </si>
   <si>
     <t xml:space="preserve">Liechtenstein.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARGN06</t>
   </si>
   <si>
     <t xml:space="preserve">FRANCOIS II</t>
@@ -398,21 +602,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L65" activeCellId="0" sqref="L65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C59" activeCellId="0" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="4.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="4.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="4.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -446,48 +651,54 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="F2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H2" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
@@ -496,433 +707,478 @@
         <v>1</v>
       </c>
       <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H3" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="F4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H4" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>3</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>3</v>
       </c>
       <c r="G5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H5" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>2</v>
+        <v>22</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>3</v>
       </c>
       <c r="G6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>2</v>
+        <v>24</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" s="0" t="n">
         <v>6.5</v>
       </c>
-      <c r="H7" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>2</v>
+        <v>26</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" s="0" t="n">
         <v>6.5</v>
       </c>
-      <c r="H8" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>2</v>
+        <v>28</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>7</v>
       </c>
       <c r="G9" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H9" s="0" t="n">
         <v>6.5</v>
       </c>
-      <c r="H9" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H14" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>2</v>
+        <v>40</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="H15" s="0" t="n">
         <v>12.5</v>
       </c>
-      <c r="H15" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H16" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D16" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>2.5</v>
+        <v>44</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>2.5</v>
       </c>
       <c r="F17" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G17" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="H17" s="0" t="n">
         <v>11.5</v>
       </c>
-      <c r="H17" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>2.5</v>
+        <v>46</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>2.5</v>
@@ -931,27 +1187,30 @@
         <v>2.5</v>
       </c>
       <c r="G18" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H18" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>5</v>
+        <v>48</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>5</v>
@@ -960,56 +1219,62 @@
         <v>5</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>0</v>
+        <v>52</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>0</v>
@@ -1021,24 +1286,27 @@
         <v>0</v>
       </c>
       <c r="H21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="0" t="n">
         <v>2.5</v>
       </c>
-      <c r="I21" s="0" t="n">
+      <c r="J21" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>0</v>
@@ -1050,24 +1318,27 @@
         <v>0</v>
       </c>
       <c r="H22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="0" t="n">
         <v>2.5</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="J22" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <v>0</v>
+        <v>57</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>0</v>
@@ -1079,24 +1350,27 @@
         <v>0</v>
       </c>
       <c r="H23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="0" t="n">
         <v>1.3</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="J23" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>0</v>
+        <v>59</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>0</v>
@@ -1108,24 +1382,27 @@
         <v>0</v>
       </c>
       <c r="H24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="J24" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>0</v>
+        <v>61</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>0</v>
@@ -1137,24 +1414,27 @@
         <v>0</v>
       </c>
       <c r="H25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I25" s="0" t="n">
+      <c r="J25" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>0</v>
@@ -1166,24 +1446,27 @@
         <v>0</v>
       </c>
       <c r="H26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="0" t="n">
         <v>2.5</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="J26" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>0</v>
@@ -1198,24 +1481,27 @@
         <v>0</v>
       </c>
       <c r="I27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="J27" s="0" t="s">
-        <v>40</v>
+      <c r="K27" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>0</v>
+        <v>69</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>0</v>
@@ -1230,24 +1516,27 @@
         <v>0</v>
       </c>
       <c r="I28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="J28" s="0" t="s">
-        <v>42</v>
+      <c r="K28" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>0</v>
+        <v>72</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>0</v>
@@ -1262,24 +1551,27 @@
         <v>0</v>
       </c>
       <c r="I29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="J29" s="0" t="s">
-        <v>44</v>
+      <c r="K29" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="0" t="n">
-        <v>0</v>
+        <v>75</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>0</v>
@@ -1294,24 +1586,27 @@
         <v>0</v>
       </c>
       <c r="I30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="J30" s="0" t="s">
-        <v>46</v>
+      <c r="K30" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="0" t="n">
-        <v>0</v>
+        <v>78</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>0</v>
@@ -1326,24 +1621,27 @@
         <v>0</v>
       </c>
       <c r="I31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="J31" s="0" t="s">
-        <v>48</v>
+      <c r="K31" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>0</v>
+        <v>81</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>0</v>
@@ -1358,82 +1656,91 @@
         <v>0</v>
       </c>
       <c r="I32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="J32" s="0" t="s">
-        <v>50</v>
+      <c r="K32" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E33" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="F33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H33" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="E34" s="0" t="n">
-        <v>0.5</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="G34" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H34" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H34" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="0" t="n">
-        <v>1</v>
+        <v>89</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1</v>
@@ -1442,462 +1749,510 @@
         <v>1</v>
       </c>
       <c r="G35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H35" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="F36" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="F36" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="G36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H36" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H36" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E37" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="F37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G37" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="G37" s="0" t="n">
+      <c r="H37" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H37" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="E38" s="0" t="n">
-        <v>2.5</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>2.5</v>
       </c>
       <c r="G38" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H38" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H38" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" s="0" t="n">
-        <v>2</v>
+        <v>97</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>3</v>
       </c>
       <c r="G39" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H39" s="0" t="n">
         <v>6.5</v>
       </c>
-      <c r="H39" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" s="0" t="n">
-        <v>2</v>
+        <v>99</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F40" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F40" s="0" t="n">
+      <c r="G40" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G40" s="0" t="n">
+      <c r="H40" s="0" t="n">
         <v>6.5</v>
       </c>
-      <c r="H40" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D41" s="0" t="n">
-        <v>2</v>
+        <v>101</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E41" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F41" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="F41" s="0" t="n">
+      <c r="G41" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G41" s="0" t="n">
+      <c r="H41" s="0" t="n">
         <v>6.5</v>
       </c>
-      <c r="H41" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D42" s="0" t="n">
-        <v>2</v>
+        <v>103</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>6</v>
       </c>
       <c r="G42" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H42" s="0" t="n">
         <v>6.5</v>
       </c>
-      <c r="H42" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="C43" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D43" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G43" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="H43" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="C44" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H44" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D44" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E44" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F44" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G44" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="H44" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="C45" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H45" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D45" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F45" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G45" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="H45" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="C46" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H46" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D46" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E46" s="0" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="F46" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G46" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="H46" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D47" s="0" t="n">
-        <v>2</v>
+        <v>113</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E47" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F47" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="F47" s="0" t="n">
+      <c r="G47" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G47" s="0" t="n">
+      <c r="H47" s="0" t="n">
         <v>12.5</v>
       </c>
-      <c r="H47" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D48" s="0" t="n">
-        <v>2</v>
+        <v>115</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E48" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F48" s="0" t="n">
         <v>2.5</v>
       </c>
-      <c r="F48" s="0" t="n">
+      <c r="G48" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G48" s="0" t="n">
+      <c r="H48" s="0" t="n">
         <v>12.5</v>
       </c>
-      <c r="H48" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="C49" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H49" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D49" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E49" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F49" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G49" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="H49" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D50" s="0" t="n">
-        <v>2.5</v>
+        <v>119</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>2.5</v>
       </c>
       <c r="F50" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G50" s="0" t="n">
         <v>4.5</v>
       </c>
-      <c r="G50" s="0" t="n">
+      <c r="H50" s="0" t="n">
         <v>11.5</v>
       </c>
-      <c r="H50" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D51" s="0" t="n">
-        <v>2.5</v>
+        <v>121</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>2.5</v>
@@ -1906,27 +2261,30 @@
         <v>2.5</v>
       </c>
       <c r="G51" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H51" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H51" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>71</v>
+        <v>122</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" s="0" t="n">
-        <v>4</v>
+        <v>123</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>4</v>
@@ -1935,27 +2293,30 @@
         <v>4</v>
       </c>
       <c r="G52" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H52" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" s="0" t="n">
-        <v>6</v>
+        <v>125</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>6</v>
@@ -1964,56 +2325,62 @@
         <v>6</v>
       </c>
       <c r="G53" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H53" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="H53" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>73</v>
+        <v>126</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D54" s="0" t="n">
-        <v>0</v>
+        <v>127</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E54" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G54" s="0" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="H54" s="0" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" s="0" t="n">
-        <v>0</v>
+        <v>129</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>0</v>
@@ -2025,24 +2392,27 @@
         <v>0</v>
       </c>
       <c r="H55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" s="0" t="n">
         <v>2.5</v>
       </c>
-      <c r="I55" s="0" t="n">
+      <c r="J55" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D56" s="0" t="n">
-        <v>0</v>
+        <v>131</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>0</v>
@@ -2054,24 +2424,27 @@
         <v>0</v>
       </c>
       <c r="H56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" s="0" t="n">
         <v>2.5</v>
       </c>
-      <c r="I56" s="0" t="n">
+      <c r="J56" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D57" s="0" t="n">
-        <v>0</v>
+        <v>133</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E57" s="0" t="n">
         <v>0</v>
@@ -2083,24 +2456,27 @@
         <v>0</v>
       </c>
       <c r="H57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" s="0" t="n">
         <v>1.3</v>
       </c>
-      <c r="I57" s="0" t="n">
+      <c r="J57" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D58" s="0" t="n">
-        <v>0</v>
+        <v>135</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>0</v>
@@ -2112,24 +2488,27 @@
         <v>0</v>
       </c>
       <c r="H58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="I58" s="0" t="n">
+      <c r="J58" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D59" s="0" t="n">
-        <v>0</v>
+        <v>137</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>0</v>
@@ -2141,24 +2520,27 @@
         <v>0</v>
       </c>
       <c r="H59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I59" s="0" t="n">
+      <c r="J59" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>79</v>
+        <v>138</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D60" s="0" t="n">
-        <v>0</v>
+        <v>139</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>0</v>
@@ -2170,24 +2552,27 @@
         <v>0</v>
       </c>
       <c r="H60" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I60" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J60" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D61" s="0" t="n">
-        <v>0</v>
+        <v>141</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>0</v>
@@ -2199,24 +2584,27 @@
         <v>0</v>
       </c>
       <c r="H61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="I61" s="0" t="n">
+      <c r="J61" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D62" s="0" t="n">
-        <v>0</v>
+        <v>143</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>0</v>
@@ -2228,24 +2616,27 @@
         <v>0</v>
       </c>
       <c r="H62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I62" s="0" t="n">
+      <c r="J62" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>82</v>
+        <v>144</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D63" s="0" t="n">
-        <v>0</v>
+        <v>145</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>0</v>
@@ -2260,24 +2651,27 @@
         <v>0</v>
       </c>
       <c r="I63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="J63" s="0" t="s">
-        <v>83</v>
+      <c r="K63" s="0" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>84</v>
+        <v>147</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D64" s="0" t="n">
-        <v>0</v>
+        <v>148</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>0</v>
@@ -2292,24 +2686,27 @@
         <v>0</v>
       </c>
       <c r="I64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="J64" s="0" t="s">
-        <v>85</v>
+      <c r="K64" s="0" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>86</v>
+        <v>150</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D65" s="0" t="n">
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>0</v>
@@ -2324,24 +2721,27 @@
         <v>0</v>
       </c>
       <c r="I65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="J65" s="0" t="s">
-        <v>87</v>
+      <c r="K65" s="0" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>88</v>
+        <v>153</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D66" s="0" t="n">
-        <v>0</v>
+        <v>154</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>0</v>
@@ -2356,24 +2756,27 @@
         <v>0</v>
       </c>
       <c r="I66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="J66" s="0" t="s">
-        <v>89</v>
+      <c r="K66" s="0" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>90</v>
+        <v>156</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D67" s="0" t="n">
-        <v>0</v>
+        <v>157</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>0</v>
@@ -2388,24 +2791,27 @@
         <v>0</v>
       </c>
       <c r="I67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="J67" s="0" t="s">
-        <v>91</v>
+      <c r="K67" s="0" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>92</v>
+        <v>159</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D68" s="0" t="n">
-        <v>0</v>
+        <v>160</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>0</v>
@@ -2420,10 +2826,13 @@
         <v>0</v>
       </c>
       <c r="I68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="J68" s="0" t="s">
-        <v>93</v>
+      <c r="K68" s="0" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>